<commit_message>
EPBDS-8990 Define runtime context properties in Datatype table.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8990_ContextPropertiesInDatatype.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8990_ContextPropertiesInDatatype.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-8990_ContextInTypesSupport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-8990_ContextPropertiesInDatatype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6E86D6-D521-4CB2-A578-45CA9226061C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E3CC35-3A5F-47C6-B55E-82C2902EB295}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4973" yWindow="2813" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="65">
   <si>
     <t>Rule</t>
   </si>
@@ -113,46 +113,109 @@
     <t>String</t>
   </si>
   <si>
+    <t>= Hello(1)</t>
+  </si>
+  <si>
+    <t>Test Main MainTest</t>
+  </si>
+  <si>
+    <t>Mydatatype</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Step2</t>
+  </si>
+  <si>
+    <t>= $Step1.$Step1</t>
+  </si>
+  <si>
+    <t>_res_.$Step2</t>
+  </si>
+  <si>
+    <t>Step3</t>
+  </si>
+  <si>
+    <t>Step4</t>
+  </si>
+  <si>
+    <t>= MySpr(myDatatype).$Step1</t>
+  </si>
+  <si>
+    <t>_res_.$Step4</t>
+  </si>
+  <si>
+    <t>= myDatatype.state = "AZ"</t>
+  </si>
+  <si>
+    <t>state:context.usState</t>
+  </si>
+  <si>
+    <t>myDatatype.state</t>
+  </si>
+  <si>
+    <t>Datatype MyDatatype2</t>
+  </si>
+  <si>
+    <t>state2 :context.usState</t>
+  </si>
+  <si>
+    <t>state3: context.usState</t>
+  </si>
+  <si>
+    <t>state4: context. usState</t>
+  </si>
+  <si>
+    <t>state5: context. usState</t>
+  </si>
+  <si>
+    <t>state6 :context. usState</t>
+  </si>
+  <si>
+    <t>state7 :context .usState</t>
+  </si>
+  <si>
+    <t>state8 : context .usState</t>
+  </si>
+  <si>
+    <t>state9 : context. usState</t>
+  </si>
+  <si>
+    <t>state10: context . usState</t>
+  </si>
+  <si>
+    <t>state11 :context . usState</t>
+  </si>
+  <si>
+    <t>state12:context . usState</t>
+  </si>
+  <si>
     <t>usState : context</t>
   </si>
   <si>
-    <t>= Hello(1)</t>
-  </si>
-  <si>
-    <t>Test Main MainTest</t>
-  </si>
-  <si>
-    <t>Mydatatype</t>
-  </si>
-  <si>
-    <t>Result</t>
+    <t>= myDatatype.usState = "AZ"</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult Main3(MyDatatype3 myDatatype)</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult MySpr3(MyDatatype3 myDatatype)</t>
+  </si>
+  <si>
+    <t>= MySpr3(myDatatype)</t>
+  </si>
+  <si>
+    <t>= MySpr3(myDatatype).$Step1</t>
+  </si>
+  <si>
+    <t>Test Main3 Main3Test</t>
   </si>
   <si>
     <t>myDatatype.usState</t>
   </si>
   <si>
-    <t>Step2</t>
-  </si>
-  <si>
-    <t>= $Step1.$Step1</t>
-  </si>
-  <si>
-    <t>_res_.$Step2</t>
-  </si>
-  <si>
-    <t>Step3</t>
-  </si>
-  <si>
-    <t>= myDatatype.usState = "AZ"</t>
-  </si>
-  <si>
-    <t>Step4</t>
-  </si>
-  <si>
-    <t>= MySpr(myDatatype).$Step1</t>
-  </si>
-  <si>
-    <t>_res_.$Step4</t>
+    <t>Datatype MyDatatype3</t>
   </si>
 </sst>
 </file>
@@ -574,18 +637,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF7A558-3946-426A-8A43-477C4C887725}">
-  <dimension ref="A4:F55"/>
+  <dimension ref="A4:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="24.06640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="17" t="s">
         <v>17</v>
       </c>
@@ -593,7 +656,7 @@
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
@@ -605,7 +668,7 @@
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,7 +682,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>3</v>
@@ -631,7 +694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -643,7 +706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
@@ -671,7 +734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
@@ -685,7 +748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
@@ -699,7 +762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
@@ -713,13 +776,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="17" t="s">
         <v>17</v>
       </c>
@@ -727,7 +790,7 @@
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>20</v>
       </c>
@@ -739,7 +802,7 @@
       </c>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>3</v>
@@ -765,7 +828,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
         <v>15</v>
@@ -777,7 +840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +854,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
@@ -805,7 +868,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>10</v>
       </c>
@@ -819,7 +882,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
@@ -833,7 +896,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
@@ -847,18 +910,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="12"/>
       <c r="C29" s="11"/>
       <c r="D29" s="10"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>22</v>
       </c>
@@ -866,21 +929,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="12"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" s="12" t="s">
         <v>22</v>
       </c>
@@ -888,7 +951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" s="12" t="s">
         <v>24</v>
       </c>
@@ -896,39 +959,39 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="12"/>
       <c r="B43" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -936,7 +999,7 @@
       <c r="E45" s="12"/>
       <c r="F45" s="12"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
@@ -944,7 +1007,7 @@
       <c r="E46" s="12"/>
       <c r="F46" s="12"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -952,7 +1015,7 @@
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -960,7 +1023,7 @@
       <c r="E48" s="12"/>
       <c r="F48" s="12"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
@@ -968,35 +1031,35 @@
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B51" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" s="12"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B52" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="12"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B52" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B53" s="12" t="s">
+      <c r="C53" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C53" s="12" t="s">
-        <v>34</v>
-      </c>
       <c r="D53" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>19</v>
       </c>
@@ -1007,7 +1070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>18</v>
       </c>
@@ -1017,6 +1080,247 @@
       <c r="D55" s="12" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B61" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B62" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B63" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B68" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B69" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B70" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B71" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B72" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C72" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B73" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B89" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B90" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E90" s="12"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B91" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E91" s="12"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B92" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E92" s="12"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B93" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E93" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1029,25 +1333,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB2C2B0-A6B6-4D9C-AF3D-AA7665971633}">
-  <dimension ref="B4:C5"/>
+  <dimension ref="B4:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="12"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-9313 Show error message if the same RuntimeContext properties are defined on the same level
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8990_ContextPropertiesInDatatype.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8990_ContextPropertiesInDatatype.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-8990_ContextPropertiesInDatatype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E3CC35-3A5F-47C6-B55E-82C2902EB295}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7984CA6-D061-4872-9B9E-E0170E601068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="53">
   <si>
     <t>Rule</t>
   </si>
@@ -153,42 +153,6 @@
   </si>
   <si>
     <t>myDatatype.state</t>
-  </si>
-  <si>
-    <t>Datatype MyDatatype2</t>
-  </si>
-  <si>
-    <t>state2 :context.usState</t>
-  </si>
-  <si>
-    <t>state3: context.usState</t>
-  </si>
-  <si>
-    <t>state4: context. usState</t>
-  </si>
-  <si>
-    <t>state5: context. usState</t>
-  </si>
-  <si>
-    <t>state6 :context. usState</t>
-  </si>
-  <si>
-    <t>state7 :context .usState</t>
-  </si>
-  <si>
-    <t>state8 : context .usState</t>
-  </si>
-  <si>
-    <t>state9 : context. usState</t>
-  </si>
-  <si>
-    <t>state10: context . usState</t>
-  </si>
-  <si>
-    <t>state11 :context . usState</t>
-  </si>
-  <si>
-    <t>state12:context . usState</t>
   </si>
   <si>
     <t>usState : context</t>
@@ -222,7 +186,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -247,7 +210,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -639,13 +602,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF7A558-3946-426A-8A43-477C4C887725}">
   <dimension ref="A4:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="2" max="2" width="24" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1083,7 +1046,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B61" s="12" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
@@ -1142,7 +1105,7 @@
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" s="12" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
@@ -1165,7 +1128,7 @@
         <v>24</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
@@ -1187,7 +1150,7 @@
         <v>37</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
@@ -1198,7 +1161,7 @@
         <v>38</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
@@ -1268,7 +1231,7 @@
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B89" s="12" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
@@ -1276,7 +1239,7 @@
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B90" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>36</v>
@@ -1333,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB2C2B0-A6B6-4D9C-AF3D-AA7665971633}">
-  <dimension ref="B4:C23"/>
+  <dimension ref="B4:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1356,7 +1319,7 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C7" s="12"/>
     </row>
@@ -1365,109 +1328,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="C11" s="12"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-9553 Add a test when the first field hasn't mapping to context field
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8990_ContextPropertiesInDatatype.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8990_ContextPropertiesInDatatype.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7984CA6-D061-4872-9B9E-E0170E601068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064BBD87-73B0-44EA-971A-EFC4EE8F17DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
   <si>
     <t>Rule</t>
   </si>
@@ -180,24 +180,59 @@
   </si>
   <si>
     <t>Datatype MyDatatype3</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>bla</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>requestDate : context</t>
+  </si>
+  <si>
+    <t>Datatype MyDatatype2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -209,8 +244,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -236,8 +275,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle name="Datatype" xfId="2" xr:uid="{053F9513-B522-4CE3-86B7-785A44D91A5F}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{4BB3D671-183A-4770-9AB9-5F65F9E1B6DE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -602,7 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF7A558-3946-426A-8A43-477C4C887725}">
   <dimension ref="A4:F93"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
@@ -1296,20 +1337,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB2C2B0-A6B6-4D9C-AF3D-AA7665971633}">
-  <dimension ref="B4:C8"/>
+  <dimension ref="A4:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>29</v>
       </c>
@@ -1317,19 +1362,146 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="12"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>44</v>
       </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>